<commit_message>
Finalizado os testes da pesquisa
</commit_message>
<xml_diff>
--- a/Pos_Qualys/Results_TSF+AMRF.xlsx
+++ b/Pos_Qualys/Results_TSF+AMRF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DS\tsc_box\Pos_Qualys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E266D5-7277-4E26-AEEC-0F2AF0197C75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3086FB11-8320-49BA-B3C6-8458162A0CED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{757038F8-B59C-40A8-9A44-7BB14EFB6255}"/>
   </bookViews>
@@ -636,13 +636,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF21F34-1E6B-4483-849D-3DAF6209762D}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>